<commit_message>
results rnn sissim fixed
</commit_message>
<xml_diff>
--- a/results/test_only_rnn.xlsx
+++ b/results/test_only_rnn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\שנה ג\סדנה למידה עמוקה\results\only rnn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B646C34B-B0E1-46C8-B978-375F89CFEDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995A78A3-6022-46B6-B91F-027ED9BC3DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>orig_sizes</t>
   </si>
@@ -235,85 +235,13 @@
   </si>
   <si>
     <t>psnr_16</t>
-  </si>
-  <si>
-    <t>sissim_1</t>
-  </si>
-  <si>
-    <t>sissim_2</t>
-  </si>
-  <si>
-    <t>sissim_3</t>
-  </si>
-  <si>
-    <t>sissim_4</t>
-  </si>
-  <si>
-    <t>sissim_5</t>
-  </si>
-  <si>
-    <t>sissim_6</t>
-  </si>
-  <si>
-    <t>sissim_7</t>
-  </si>
-  <si>
-    <t>sissim_8</t>
-  </si>
-  <si>
-    <t>sissim_9</t>
-  </si>
-  <si>
-    <t>sissim_10</t>
-  </si>
-  <si>
-    <t>sissim_11</t>
-  </si>
-  <si>
-    <t>sissim_12</t>
-  </si>
-  <si>
-    <t>sissim_13</t>
-  </si>
-  <si>
-    <t>sissim_14</t>
-  </si>
-  <si>
-    <t>sissim_15</t>
-  </si>
-  <si>
-    <t>sissim_16</t>
-  </si>
-  <si>
-    <t>sissim_17</t>
-  </si>
-  <si>
-    <t>sissim_18</t>
-  </si>
-  <si>
-    <t>sissim_19</t>
-  </si>
-  <si>
-    <t>sissim_20</t>
-  </si>
-  <si>
-    <t>sissim_21</t>
-  </si>
-  <si>
-    <t>sissim_22</t>
-  </si>
-  <si>
-    <t>sissim_23</t>
-  </si>
-  <si>
-    <t>sissim_24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,17 +262,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -354,7 +271,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -377,26 +294,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -405,10 +307,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,18 +645,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CN28"/>
+  <dimension ref="A1:BP26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="CM27" sqref="CM27"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BI13" sqref="BI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="69" max="92" width="8.44140625" style="2" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,80 +855,8 @@
       <c r="BP1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BQ1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="BZ1" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="CA1" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="CB1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC1" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="CF1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="CG1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH1" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="CJ1" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CK1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="CL1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="CN1" s="4" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="2" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1238,80 +1061,8 @@
       <c r="BP2" s="2">
         <v>29.97116851806641</v>
       </c>
-      <c r="BQ2" s="5">
-        <v>0.4330480694770813</v>
-      </c>
-      <c r="BR2" s="5">
-        <v>0.53977036476135254</v>
-      </c>
-      <c r="BS2" s="5">
-        <v>0.62532311677932739</v>
-      </c>
-      <c r="BT2" s="5">
-        <v>0.69178128242492676</v>
-      </c>
-      <c r="BU2" s="5">
-        <v>0.74050581455230713</v>
-      </c>
-      <c r="BV2" s="5">
-        <v>0.77717369794845581</v>
-      </c>
-      <c r="BW2" s="5">
-        <v>0.80442929267883301</v>
-      </c>
-      <c r="BX2" s="5">
-        <v>0.8242037296295166</v>
-      </c>
-      <c r="BY2" s="5">
-        <v>0.84097695350646973</v>
-      </c>
-      <c r="BZ2" s="5">
-        <v>0.85307276248931885</v>
-      </c>
-      <c r="CA2" s="5">
-        <v>0.86290085315704346</v>
-      </c>
-      <c r="CB2" s="5">
-        <v>0.86962741613388062</v>
-      </c>
-      <c r="CC2" s="5">
-        <v>0.87637478113174438</v>
-      </c>
-      <c r="CD2" s="5">
-        <v>0.88209319114685059</v>
-      </c>
-      <c r="CE2" s="5">
-        <v>0.88616615533828735</v>
-      </c>
-      <c r="CF2" s="5">
-        <v>0.88906234502792358</v>
-      </c>
-      <c r="CG2" s="5">
-        <v>0.89099925756454468</v>
-      </c>
-      <c r="CH2" s="5">
-        <v>0.89309340715408325</v>
-      </c>
-      <c r="CI2" s="5">
-        <v>0.89503055810928345</v>
-      </c>
-      <c r="CJ2" s="5">
-        <v>0.89659571647644043</v>
-      </c>
-      <c r="CK2" s="5">
-        <v>0.89879786968231201</v>
-      </c>
-      <c r="CL2" s="5">
-        <v>0.90029251575469971</v>
-      </c>
-      <c r="CM2" s="5">
-        <v>0.90157783031463623</v>
-      </c>
-      <c r="CN2" s="5">
-        <v>0.90244418382644653</v>
-      </c>
     </row>
-    <row r="3" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1516,80 +1267,8 @@
       <c r="BP3" s="2">
         <v>33.564788818359382</v>
       </c>
-      <c r="BQ3" s="5">
-        <v>0.61680805683135986</v>
-      </c>
-      <c r="BR3" s="5">
-        <v>0.68877965211868286</v>
-      </c>
-      <c r="BS3" s="5">
-        <v>0.72270846366882324</v>
-      </c>
-      <c r="BT3" s="5">
-        <v>0.75325340032577515</v>
-      </c>
-      <c r="BU3" s="5">
-        <v>0.78409713506698608</v>
-      </c>
-      <c r="BV3" s="5">
-        <v>0.80920809507369995</v>
-      </c>
-      <c r="BW3" s="5">
-        <v>0.824474036693573</v>
-      </c>
-      <c r="BX3" s="5">
-        <v>0.83824336528778076</v>
-      </c>
-      <c r="BY3" s="5">
-        <v>0.84844028949737549</v>
-      </c>
-      <c r="BZ3" s="5">
-        <v>0.8545871376991272</v>
-      </c>
-      <c r="CA3" s="5">
-        <v>0.85986530780792236</v>
-      </c>
-      <c r="CB3" s="5">
-        <v>0.86458075046539307</v>
-      </c>
-      <c r="CC3" s="5">
-        <v>0.86877155303955078</v>
-      </c>
-      <c r="CD3" s="5">
-        <v>0.87279409170150757</v>
-      </c>
-      <c r="CE3" s="5">
-        <v>0.8756137490272522</v>
-      </c>
-      <c r="CF3" s="5">
-        <v>0.87796527147293091</v>
-      </c>
-      <c r="CG3" s="5">
-        <v>0.87911105155944824</v>
-      </c>
-      <c r="CH3" s="5">
-        <v>0.88053566217422485</v>
-      </c>
-      <c r="CI3" s="5">
-        <v>0.88132905960083008</v>
-      </c>
-      <c r="CJ3" s="5">
-        <v>0.88247179985046387</v>
-      </c>
-      <c r="CK3" s="5">
-        <v>0.88366222381591797</v>
-      </c>
-      <c r="CL3" s="5">
-        <v>0.88491219282150269</v>
-      </c>
-      <c r="CM3" s="5">
-        <v>0.88590061664581299</v>
-      </c>
-      <c r="CN3" s="5">
-        <v>0.88670289516448975</v>
-      </c>
     </row>
-    <row r="4" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1794,80 +1473,8 @@
       <c r="BP4" s="2">
         <v>35.18243408203125</v>
       </c>
-      <c r="BQ4" s="5">
-        <v>0.74179339408874512</v>
-      </c>
-      <c r="BR4" s="5">
-        <v>0.79734009504318237</v>
-      </c>
-      <c r="BS4" s="5">
-        <v>0.82676172256469727</v>
-      </c>
-      <c r="BT4" s="5">
-        <v>0.84932798147201538</v>
-      </c>
-      <c r="BU4" s="5">
-        <v>0.86830174922943115</v>
-      </c>
-      <c r="BV4" s="5">
-        <v>0.88411915302276611</v>
-      </c>
-      <c r="BW4" s="5">
-        <v>0.89410483837127686</v>
-      </c>
-      <c r="BX4" s="5">
-        <v>0.90280407667160034</v>
-      </c>
-      <c r="BY4" s="5">
-        <v>0.9093477725982666</v>
-      </c>
-      <c r="BZ4" s="5">
-        <v>0.91382300853729248</v>
-      </c>
-      <c r="CA4" s="5">
-        <v>0.91726577281951904</v>
-      </c>
-      <c r="CB4" s="5">
-        <v>0.92036682367324829</v>
-      </c>
-      <c r="CC4" s="5">
-        <v>0.92306870222091675</v>
-      </c>
-      <c r="CD4" s="5">
-        <v>0.9253537654876709</v>
-      </c>
-      <c r="CE4" s="5">
-        <v>0.92657065391540527</v>
-      </c>
-      <c r="CF4" s="5">
-        <v>0.9277682900428772</v>
-      </c>
-      <c r="CG4" s="5">
-        <v>0.92854142189025879</v>
-      </c>
-      <c r="CH4" s="5">
-        <v>0.92923027276992798</v>
-      </c>
-      <c r="CI4" s="5">
-        <v>0.92984557151794434</v>
-      </c>
-      <c r="CJ4" s="5">
-        <v>0.93036150932312012</v>
-      </c>
-      <c r="CK4" s="5">
-        <v>0.93127375841140747</v>
-      </c>
-      <c r="CL4" s="5">
-        <v>0.93211627006530762</v>
-      </c>
-      <c r="CM4" s="5">
-        <v>0.93253582715988159</v>
-      </c>
-      <c r="CN4" s="5">
-        <v>0.93289065361022949</v>
-      </c>
     </row>
-    <row r="5" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2072,80 +1679,8 @@
       <c r="BP5" s="2">
         <v>33.823799133300781</v>
       </c>
-      <c r="BQ5" s="5">
-        <v>0.65796637535095215</v>
-      </c>
-      <c r="BR5" s="5">
-        <v>0.71877259016036987</v>
-      </c>
-      <c r="BS5" s="5">
-        <v>0.75442087650299072</v>
-      </c>
-      <c r="BT5" s="5">
-        <v>0.78727442026138306</v>
-      </c>
-      <c r="BU5" s="5">
-        <v>0.81402570009231567</v>
-      </c>
-      <c r="BV5" s="5">
-        <v>0.83543699979782104</v>
-      </c>
-      <c r="BW5" s="5">
-        <v>0.85127371549606323</v>
-      </c>
-      <c r="BX5" s="5">
-        <v>0.8637121319770813</v>
-      </c>
-      <c r="BY5" s="5">
-        <v>0.87264823913574219</v>
-      </c>
-      <c r="BZ5" s="5">
-        <v>0.87893736362457275</v>
-      </c>
-      <c r="CA5" s="5">
-        <v>0.88412666320800781</v>
-      </c>
-      <c r="CB5" s="5">
-        <v>0.88845992088317871</v>
-      </c>
-      <c r="CC5" s="5">
-        <v>0.89202296733856201</v>
-      </c>
-      <c r="CD5" s="5">
-        <v>0.89532214403152466</v>
-      </c>
-      <c r="CE5" s="5">
-        <v>0.89800208806991577</v>
-      </c>
-      <c r="CF5" s="5">
-        <v>0.89990085363388062</v>
-      </c>
-      <c r="CG5" s="5">
-        <v>0.90097641944885254</v>
-      </c>
-      <c r="CH5" s="5">
-        <v>0.90207457542419434</v>
-      </c>
-      <c r="CI5" s="5">
-        <v>0.90322387218475342</v>
-      </c>
-      <c r="CJ5" s="5">
-        <v>0.90417277812957764</v>
-      </c>
-      <c r="CK5" s="5">
-        <v>0.90537440776824951</v>
-      </c>
-      <c r="CL5" s="5">
-        <v>0.90652728080749512</v>
-      </c>
-      <c r="CM5" s="5">
-        <v>0.90722477436065674</v>
-      </c>
-      <c r="CN5" s="5">
-        <v>0.90783035755157471</v>
-      </c>
     </row>
-    <row r="6" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2350,80 +1885,8 @@
       <c r="BP6" s="2">
         <v>29.522159576416019</v>
       </c>
-      <c r="BQ6" s="5">
-        <v>0.47863829135894781</v>
-      </c>
-      <c r="BR6" s="5">
-        <v>0.60197257995605469</v>
-      </c>
-      <c r="BS6" s="5">
-        <v>0.67532515525817871</v>
-      </c>
-      <c r="BT6" s="5">
-        <v>0.72953009605407715</v>
-      </c>
-      <c r="BU6" s="5">
-        <v>0.77572166919708252</v>
-      </c>
-      <c r="BV6" s="5">
-        <v>0.81131595373153687</v>
-      </c>
-      <c r="BW6" s="5">
-        <v>0.83891564607620239</v>
-      </c>
-      <c r="BX6" s="5">
-        <v>0.8565971851348877</v>
-      </c>
-      <c r="BY6" s="5">
-        <v>0.87170571088790894</v>
-      </c>
-      <c r="BZ6" s="5">
-        <v>0.8822440505027771</v>
-      </c>
-      <c r="CA6" s="5">
-        <v>0.89044094085693359</v>
-      </c>
-      <c r="CB6" s="5">
-        <v>0.89662975072860718</v>
-      </c>
-      <c r="CC6" s="5">
-        <v>0.90226131677627563</v>
-      </c>
-      <c r="CD6" s="5">
-        <v>0.90689331293106079</v>
-      </c>
-      <c r="CE6" s="5">
-        <v>0.91018170118331909</v>
-      </c>
-      <c r="CF6" s="5">
-        <v>0.91246795654296875</v>
-      </c>
-      <c r="CG6" s="5">
-        <v>0.9140777587890625</v>
-      </c>
-      <c r="CH6" s="5">
-        <v>0.915638267993927</v>
-      </c>
-      <c r="CI6" s="5">
-        <v>0.91722732782363892</v>
-      </c>
-      <c r="CJ6" s="5">
-        <v>0.91833806037902832</v>
-      </c>
-      <c r="CK6" s="5">
-        <v>0.91984200477600098</v>
-      </c>
-      <c r="CL6" s="5">
-        <v>0.92082047462463379</v>
-      </c>
-      <c r="CM6" s="5">
-        <v>0.92188751697540283</v>
-      </c>
-      <c r="CN6" s="5">
-        <v>0.92252647876739502</v>
-      </c>
     </row>
-    <row r="7" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2628,80 +2091,8 @@
       <c r="BP7" s="2">
         <v>30.9461669921875</v>
       </c>
-      <c r="BQ7" s="5">
-        <v>0.5307915210723877</v>
-      </c>
-      <c r="BR7" s="5">
-        <v>0.60572373867034912</v>
-      </c>
-      <c r="BS7" s="5">
-        <v>0.67004501819610596</v>
-      </c>
-      <c r="BT7" s="5">
-        <v>0.72760856151580811</v>
-      </c>
-      <c r="BU7" s="5">
-        <v>0.76950091123580933</v>
-      </c>
-      <c r="BV7" s="5">
-        <v>0.80429732799530029</v>
-      </c>
-      <c r="BW7" s="5">
-        <v>0.83000266551971436</v>
-      </c>
-      <c r="BX7" s="5">
-        <v>0.8457685112953186</v>
-      </c>
-      <c r="BY7" s="5">
-        <v>0.86257100105285645</v>
-      </c>
-      <c r="BZ7" s="5">
-        <v>0.87418824434280396</v>
-      </c>
-      <c r="CA7" s="5">
-        <v>0.88219523429870605</v>
-      </c>
-      <c r="CB7" s="5">
-        <v>0.88818037509918213</v>
-      </c>
-      <c r="CC7" s="5">
-        <v>0.89365184307098389</v>
-      </c>
-      <c r="CD7" s="5">
-        <v>0.8978620171546936</v>
-      </c>
-      <c r="CE7" s="5">
-        <v>0.90104377269744873</v>
-      </c>
-      <c r="CF7" s="5">
-        <v>0.90307354927062988</v>
-      </c>
-      <c r="CG7" s="5">
-        <v>0.90468817949295044</v>
-      </c>
-      <c r="CH7" s="5">
-        <v>0.9062151312828064</v>
-      </c>
-      <c r="CI7" s="5">
-        <v>0.90776658058166504</v>
-      </c>
-      <c r="CJ7" s="5">
-        <v>0.90870761871337891</v>
-      </c>
-      <c r="CK7" s="5">
-        <v>0.91003471612930298</v>
-      </c>
-      <c r="CL7" s="5">
-        <v>0.91099274158477783</v>
-      </c>
-      <c r="CM7" s="5">
-        <v>0.91194301843643188</v>
-      </c>
-      <c r="CN7" s="5">
-        <v>0.91263836622238159</v>
-      </c>
     </row>
-    <row r="8" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2906,80 +2297,8 @@
       <c r="BP8" s="2">
         <v>34.852123260498047</v>
       </c>
-      <c r="BQ8" s="5">
-        <v>0.73295527696609497</v>
-      </c>
-      <c r="BR8" s="5">
-        <v>0.82388436794281006</v>
-      </c>
-      <c r="BS8" s="5">
-        <v>0.86388993263244629</v>
-      </c>
-      <c r="BT8" s="5">
-        <v>0.88918429613113403</v>
-      </c>
-      <c r="BU8" s="5">
-        <v>0.90621227025985718</v>
-      </c>
-      <c r="BV8" s="5">
-        <v>0.91787624359130859</v>
-      </c>
-      <c r="BW8" s="5">
-        <v>0.92575579881668091</v>
-      </c>
-      <c r="BX8" s="5">
-        <v>0.9317811131477356</v>
-      </c>
-      <c r="BY8" s="5">
-        <v>0.93566989898681641</v>
-      </c>
-      <c r="BZ8" s="5">
-        <v>0.9387284517288208</v>
-      </c>
-      <c r="CA8" s="5">
-        <v>0.94103336334228516</v>
-      </c>
-      <c r="CB8" s="5">
-        <v>0.94279831647872925</v>
-      </c>
-      <c r="CC8" s="5">
-        <v>0.94462692737579346</v>
-      </c>
-      <c r="CD8" s="5">
-        <v>0.94615429639816284</v>
-      </c>
-      <c r="CE8" s="5">
-        <v>0.94720840454101563</v>
-      </c>
-      <c r="CF8" s="5">
-        <v>0.94795483350753784</v>
-      </c>
-      <c r="CG8" s="5">
-        <v>0.94841068983078003</v>
-      </c>
-      <c r="CH8" s="5">
-        <v>0.94890362024307251</v>
-      </c>
-      <c r="CI8" s="5">
-        <v>0.94928401708602905</v>
-      </c>
-      <c r="CJ8" s="5">
-        <v>0.94966357946395874</v>
-      </c>
-      <c r="CK8" s="5">
-        <v>0.9500424861907959</v>
-      </c>
-      <c r="CL8" s="5">
-        <v>0.95046085119247437</v>
-      </c>
-      <c r="CM8" s="5">
-        <v>0.95079547166824341</v>
-      </c>
-      <c r="CN8" s="5">
-        <v>0.95107924938201904</v>
-      </c>
     </row>
-    <row r="9" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3184,80 +2503,8 @@
       <c r="BP9" s="2">
         <v>28.28458404541016</v>
       </c>
-      <c r="BQ9" s="5">
-        <v>0.46657153964042658</v>
-      </c>
-      <c r="BR9" s="5">
-        <v>0.56943368911743164</v>
-      </c>
-      <c r="BS9" s="5">
-        <v>0.6468157172203064</v>
-      </c>
-      <c r="BT9" s="5">
-        <v>0.71254414319992065</v>
-      </c>
-      <c r="BU9" s="5">
-        <v>0.76282477378845215</v>
-      </c>
-      <c r="BV9" s="5">
-        <v>0.80013644695281982</v>
-      </c>
-      <c r="BW9" s="5">
-        <v>0.82615447044372559</v>
-      </c>
-      <c r="BX9" s="5">
-        <v>0.84397375583648682</v>
-      </c>
-      <c r="BY9" s="5">
-        <v>0.85886931419372559</v>
-      </c>
-      <c r="BZ9" s="5">
-        <v>0.86824244260787964</v>
-      </c>
-      <c r="CA9" s="5">
-        <v>0.87737536430358887</v>
-      </c>
-      <c r="CB9" s="5">
-        <v>0.88276046514511108</v>
-      </c>
-      <c r="CC9" s="5">
-        <v>0.88778084516525269</v>
-      </c>
-      <c r="CD9" s="5">
-        <v>0.89267414808273315</v>
-      </c>
-      <c r="CE9" s="5">
-        <v>0.89653885364532471</v>
-      </c>
-      <c r="CF9" s="5">
-        <v>0.8991696834564209</v>
-      </c>
-      <c r="CG9" s="5">
-        <v>0.90114188194274902</v>
-      </c>
-      <c r="CH9" s="5">
-        <v>0.90297669172286987</v>
-      </c>
-      <c r="CI9" s="5">
-        <v>0.9051743745803833</v>
-      </c>
-      <c r="CJ9" s="5">
-        <v>0.90651363134384155</v>
-      </c>
-      <c r="CK9" s="5">
-        <v>0.90829002857208252</v>
-      </c>
-      <c r="CL9" s="5">
-        <v>0.90956223011016846</v>
-      </c>
-      <c r="CM9" s="5">
-        <v>0.91115528345108032</v>
-      </c>
-      <c r="CN9" s="5">
-        <v>0.9119417667388916</v>
-      </c>
     </row>
-    <row r="10" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3462,80 +2709,8 @@
       <c r="BP10" s="2">
         <v>35.086189270019531</v>
       </c>
-      <c r="BQ10" s="5">
-        <v>0.73990428447723389</v>
-      </c>
-      <c r="BR10" s="5">
-        <v>0.80014985799789429</v>
-      </c>
-      <c r="BS10" s="5">
-        <v>0.83790171146392822</v>
-      </c>
-      <c r="BT10" s="5">
-        <v>0.86367744207382202</v>
-      </c>
-      <c r="BU10" s="5">
-        <v>0.87986218929290771</v>
-      </c>
-      <c r="BV10" s="5">
-        <v>0.89273643493652344</v>
-      </c>
-      <c r="BW10" s="5">
-        <v>0.90092533826828003</v>
-      </c>
-      <c r="BX10" s="5">
-        <v>0.90700793266296387</v>
-      </c>
-      <c r="BY10" s="5">
-        <v>0.91143447160720825</v>
-      </c>
-      <c r="BZ10" s="5">
-        <v>0.91477924585342407</v>
-      </c>
-      <c r="CA10" s="5">
-        <v>0.91724175214767456</v>
-      </c>
-      <c r="CB10" s="5">
-        <v>0.9192659854888916</v>
-      </c>
-      <c r="CC10" s="5">
-        <v>0.9211307168006897</v>
-      </c>
-      <c r="CD10" s="5">
-        <v>0.92257130146026611</v>
-      </c>
-      <c r="CE10" s="5">
-        <v>0.92367255687713623</v>
-      </c>
-      <c r="CF10" s="5">
-        <v>0.92455810308456421</v>
-      </c>
-      <c r="CG10" s="5">
-        <v>0.92504608631134033</v>
-      </c>
-      <c r="CH10" s="5">
-        <v>0.92560452222824097</v>
-      </c>
-      <c r="CI10" s="5">
-        <v>0.92618262767791748</v>
-      </c>
-      <c r="CJ10" s="5">
-        <v>0.92662239074707031</v>
-      </c>
-      <c r="CK10" s="5">
-        <v>0.92707908153533936</v>
-      </c>
-      <c r="CL10" s="5">
-        <v>0.92747223377227783</v>
-      </c>
-      <c r="CM10" s="5">
-        <v>0.92774432897567749</v>
-      </c>
-      <c r="CN10" s="5">
-        <v>0.92806136608123779</v>
-      </c>
     </row>
-    <row r="11" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3740,80 +2915,8 @@
       <c r="BP11" s="2">
         <v>34.792942047119141</v>
       </c>
-      <c r="BQ11" s="5">
-        <v>0.70959126949310303</v>
-      </c>
-      <c r="BR11" s="5">
-        <v>0.77335703372955322</v>
-      </c>
-      <c r="BS11" s="5">
-        <v>0.81429886817932129</v>
-      </c>
-      <c r="BT11" s="5">
-        <v>0.84686213731765747</v>
-      </c>
-      <c r="BU11" s="5">
-        <v>0.86892193555831909</v>
-      </c>
-      <c r="BV11" s="5">
-        <v>0.88441777229309082</v>
-      </c>
-      <c r="BW11" s="5">
-        <v>0.89480197429656982</v>
-      </c>
-      <c r="BX11" s="5">
-        <v>0.90238475799560547</v>
-      </c>
-      <c r="BY11" s="5">
-        <v>0.90767860412597656</v>
-      </c>
-      <c r="BZ11" s="5">
-        <v>0.91123050451278687</v>
-      </c>
-      <c r="CA11" s="5">
-        <v>0.91443485021591187</v>
-      </c>
-      <c r="CB11" s="5">
-        <v>0.91658169031143188</v>
-      </c>
-      <c r="CC11" s="5">
-        <v>0.91860079765319824</v>
-      </c>
-      <c r="CD11" s="5">
-        <v>0.92056971788406372</v>
-      </c>
-      <c r="CE11" s="5">
-        <v>0.92170947790145874</v>
-      </c>
-      <c r="CF11" s="5">
-        <v>0.92285168170928955</v>
-      </c>
-      <c r="CG11" s="5">
-        <v>0.92336052656173706</v>
-      </c>
-      <c r="CH11" s="5">
-        <v>0.92379939556121826</v>
-      </c>
-      <c r="CI11" s="5">
-        <v>0.92452800273895264</v>
-      </c>
-      <c r="CJ11" s="5">
-        <v>0.92486751079559326</v>
-      </c>
-      <c r="CK11" s="5">
-        <v>0.92537236213684082</v>
-      </c>
-      <c r="CL11" s="5">
-        <v>0.92594349384307861</v>
-      </c>
-      <c r="CM11" s="5">
-        <v>0.92633777856826782</v>
-      </c>
-      <c r="CN11" s="5">
-        <v>0.9266316294670105</v>
-      </c>
     </row>
-    <row r="12" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -4018,80 +3121,8 @@
       <c r="BP12" s="2">
         <v>31.82027626037598</v>
       </c>
-      <c r="BQ12" s="5">
-        <v>0.57159042358398438</v>
-      </c>
-      <c r="BR12" s="5">
-        <v>0.65492582321166992</v>
-      </c>
-      <c r="BS12" s="5">
-        <v>0.70594882965087891</v>
-      </c>
-      <c r="BT12" s="5">
-        <v>0.7530398964881897</v>
-      </c>
-      <c r="BU12" s="5">
-        <v>0.7900509238243103</v>
-      </c>
-      <c r="BV12" s="5">
-        <v>0.81915634870529175</v>
-      </c>
-      <c r="BW12" s="5">
-        <v>0.83948016166687012</v>
-      </c>
-      <c r="BX12" s="5">
-        <v>0.85352230072021484</v>
-      </c>
-      <c r="BY12" s="5">
-        <v>0.866554856300354</v>
-      </c>
-      <c r="BZ12" s="5">
-        <v>0.87469106912612915</v>
-      </c>
-      <c r="CA12" s="5">
-        <v>0.88115626573562622</v>
-      </c>
-      <c r="CB12" s="5">
-        <v>0.88646954298019409</v>
-      </c>
-      <c r="CC12" s="5">
-        <v>0.89120906591415405</v>
-      </c>
-      <c r="CD12" s="5">
-        <v>0.89523476362228394</v>
-      </c>
-      <c r="CE12" s="5">
-        <v>0.89832901954650879</v>
-      </c>
-      <c r="CF12" s="5">
-        <v>0.90011203289031982</v>
-      </c>
-      <c r="CG12" s="5">
-        <v>0.90166878700256348</v>
-      </c>
-      <c r="CH12" s="5">
-        <v>0.903278648853302</v>
-      </c>
-      <c r="CI12" s="5">
-        <v>0.90449988842010498</v>
-      </c>
-      <c r="CJ12" s="5">
-        <v>0.90495204925537109</v>
-      </c>
-      <c r="CK12" s="5">
-        <v>0.90660899877548218</v>
-      </c>
-      <c r="CL12" s="5">
-        <v>0.90756773948669434</v>
-      </c>
-      <c r="CM12" s="5">
-        <v>0.90844333171844482</v>
-      </c>
-      <c r="CN12" s="5">
-        <v>0.90897494554519653</v>
-      </c>
     </row>
-    <row r="13" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -4296,80 +3327,8 @@
       <c r="BP13" s="2">
         <v>35.430736541748047</v>
       </c>
-      <c r="BQ13" s="5">
-        <v>0.70707577466964722</v>
-      </c>
-      <c r="BR13" s="5">
-        <v>0.75258976221084595</v>
-      </c>
-      <c r="BS13" s="5">
-        <v>0.78582572937011719</v>
-      </c>
-      <c r="BT13" s="5">
-        <v>0.81632733345031738</v>
-      </c>
-      <c r="BU13" s="5">
-        <v>0.84064072370529175</v>
-      </c>
-      <c r="BV13" s="5">
-        <v>0.8616788387298584</v>
-      </c>
-      <c r="BW13" s="5">
-        <v>0.87535732984542847</v>
-      </c>
-      <c r="BX13" s="5">
-        <v>0.88550776243209839</v>
-      </c>
-      <c r="BY13" s="5">
-        <v>0.89339804649353027</v>
-      </c>
-      <c r="BZ13" s="5">
-        <v>0.89854174852371216</v>
-      </c>
-      <c r="CA13" s="5">
-        <v>0.90280532836914063</v>
-      </c>
-      <c r="CB13" s="5">
-        <v>0.90660667419433594</v>
-      </c>
-      <c r="CC13" s="5">
-        <v>0.90967899560928345</v>
-      </c>
-      <c r="CD13" s="5">
-        <v>0.91234630346298218</v>
-      </c>
-      <c r="CE13" s="5">
-        <v>0.91464531421661377</v>
-      </c>
-      <c r="CF13" s="5">
-        <v>0.91606491804122925</v>
-      </c>
-      <c r="CG13" s="5">
-        <v>0.91666150093078613</v>
-      </c>
-      <c r="CH13" s="5">
-        <v>0.91752982139587402</v>
-      </c>
-      <c r="CI13" s="5">
-        <v>0.91826492547988892</v>
-      </c>
-      <c r="CJ13" s="5">
-        <v>0.91877704858779907</v>
-      </c>
-      <c r="CK13" s="5">
-        <v>0.91992229223251343</v>
-      </c>
-      <c r="CL13" s="5">
-        <v>0.92069065570831299</v>
-      </c>
-      <c r="CM13" s="5">
-        <v>0.92147308588027954</v>
-      </c>
-      <c r="CN13" s="5">
-        <v>0.92193865776062012</v>
-      </c>
     </row>
-    <row r="14" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4574,80 +3533,8 @@
       <c r="BP14" s="2">
         <v>26.416900634765621</v>
       </c>
-      <c r="BQ14" s="5">
-        <v>0.36965641379356379</v>
-      </c>
-      <c r="BR14" s="5">
-        <v>0.4671555757522583</v>
-      </c>
-      <c r="BS14" s="5">
-        <v>0.53995275497436523</v>
-      </c>
-      <c r="BT14" s="5">
-        <v>0.59975188970565796</v>
-      </c>
-      <c r="BU14" s="5">
-        <v>0.65078699588775635</v>
-      </c>
-      <c r="BV14" s="5">
-        <v>0.69506156444549561</v>
-      </c>
-      <c r="BW14" s="5">
-        <v>0.73449540138244629</v>
-      </c>
-      <c r="BX14" s="5">
-        <v>0.75987124443054199</v>
-      </c>
-      <c r="BY14" s="5">
-        <v>0.78573203086853027</v>
-      </c>
-      <c r="BZ14" s="5">
-        <v>0.80309158563613892</v>
-      </c>
-      <c r="CA14" s="5">
-        <v>0.81747448444366455</v>
-      </c>
-      <c r="CB14" s="5">
-        <v>0.82744723558425903</v>
-      </c>
-      <c r="CC14" s="5">
-        <v>0.83659052848815918</v>
-      </c>
-      <c r="CD14" s="5">
-        <v>0.84390020370483398</v>
-      </c>
-      <c r="CE14" s="5">
-        <v>0.84981584548950195</v>
-      </c>
-      <c r="CF14" s="5">
-        <v>0.85330414772033691</v>
-      </c>
-      <c r="CG14" s="5">
-        <v>0.85636669397354126</v>
-      </c>
-      <c r="CH14" s="5">
-        <v>0.8592231273651123</v>
-      </c>
-      <c r="CI14" s="5">
-        <v>0.86214756965637207</v>
-      </c>
-      <c r="CJ14" s="5">
-        <v>0.86420023441314697</v>
-      </c>
-      <c r="CK14" s="5">
-        <v>0.86660623550415039</v>
-      </c>
-      <c r="CL14" s="5">
-        <v>0.86838310956954956</v>
-      </c>
-      <c r="CM14" s="5">
-        <v>0.87000358104705811</v>
-      </c>
-      <c r="CN14" s="5">
-        <v>0.87107002735137939</v>
-      </c>
     </row>
-    <row r="15" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4852,80 +3739,8 @@
       <c r="BP15" s="2">
         <v>30.56369590759277</v>
       </c>
-      <c r="BQ15" s="5">
-        <v>0.5089295506477356</v>
-      </c>
-      <c r="BR15" s="5">
-        <v>0.6143108606338501</v>
-      </c>
-      <c r="BS15" s="5">
-        <v>0.67640775442123413</v>
-      </c>
-      <c r="BT15" s="5">
-        <v>0.72667211294174194</v>
-      </c>
-      <c r="BU15" s="5">
-        <v>0.7663300633430481</v>
-      </c>
-      <c r="BV15" s="5">
-        <v>0.79875504970550537</v>
-      </c>
-      <c r="BW15" s="5">
-        <v>0.82182943820953369</v>
-      </c>
-      <c r="BX15" s="5">
-        <v>0.83906674385070801</v>
-      </c>
-      <c r="BY15" s="5">
-        <v>0.85357153415679932</v>
-      </c>
-      <c r="BZ15" s="5">
-        <v>0.86318498849868774</v>
-      </c>
-      <c r="CA15" s="5">
-        <v>0.87059569358825684</v>
-      </c>
-      <c r="CB15" s="5">
-        <v>0.87675803899765015</v>
-      </c>
-      <c r="CC15" s="5">
-        <v>0.88221359252929688</v>
-      </c>
-      <c r="CD15" s="5">
-        <v>0.88682186603546143</v>
-      </c>
-      <c r="CE15" s="5">
-        <v>0.89014351367950439</v>
-      </c>
-      <c r="CF15" s="5">
-        <v>0.89263415336608887</v>
-      </c>
-      <c r="CG15" s="5">
-        <v>0.89416193962097168</v>
-      </c>
-      <c r="CH15" s="5">
-        <v>0.89571911096572876</v>
-      </c>
-      <c r="CI15" s="5">
-        <v>0.89718043804168701</v>
-      </c>
-      <c r="CJ15" s="5">
-        <v>0.89843302965164185</v>
-      </c>
-      <c r="CK15" s="5">
-        <v>0.90003776550292969</v>
-      </c>
-      <c r="CL15" s="5">
-        <v>0.90118134021759033</v>
-      </c>
-      <c r="CM15" s="5">
-        <v>0.90213465690612793</v>
-      </c>
-      <c r="CN15" s="5">
-        <v>0.90301346778869629</v>
-      </c>
     </row>
-    <row r="16" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -5130,80 +3945,8 @@
       <c r="BP16" s="2">
         <v>33.455005645751953</v>
       </c>
-      <c r="BQ16" s="5">
-        <v>0.65444493293762207</v>
-      </c>
-      <c r="BR16" s="5">
-        <v>0.74320858716964722</v>
-      </c>
-      <c r="BS16" s="5">
-        <v>0.78193074464797974</v>
-      </c>
-      <c r="BT16" s="5">
-        <v>0.80699276924133301</v>
-      </c>
-      <c r="BU16" s="5">
-        <v>0.82918655872344971</v>
-      </c>
-      <c r="BV16" s="5">
-        <v>0.8477858304977417</v>
-      </c>
-      <c r="BW16" s="5">
-        <v>0.86085432767868042</v>
-      </c>
-      <c r="BX16" s="5">
-        <v>0.87085628509521484</v>
-      </c>
-      <c r="BY16" s="5">
-        <v>0.87797015905380249</v>
-      </c>
-      <c r="BZ16" s="5">
-        <v>0.88327944278717041</v>
-      </c>
-      <c r="CA16" s="5">
-        <v>0.8875737190246582</v>
-      </c>
-      <c r="CB16" s="5">
-        <v>0.8911362886428833</v>
-      </c>
-      <c r="CC16" s="5">
-        <v>0.89402836561203003</v>
-      </c>
-      <c r="CD16" s="5">
-        <v>0.89728927612304688</v>
-      </c>
-      <c r="CE16" s="5">
-        <v>0.89949345588684082</v>
-      </c>
-      <c r="CF16" s="5">
-        <v>0.90083515644073486</v>
-      </c>
-      <c r="CG16" s="5">
-        <v>0.90175163745880127</v>
-      </c>
-      <c r="CH16" s="5">
-        <v>0.90267956256866455</v>
-      </c>
-      <c r="CI16" s="5">
-        <v>0.90368080139160156</v>
-      </c>
-      <c r="CJ16" s="5">
-        <v>0.90449249744415283</v>
-      </c>
-      <c r="CK16" s="5">
-        <v>0.90552669763565063</v>
-      </c>
-      <c r="CL16" s="5">
-        <v>0.906513512134552</v>
-      </c>
-      <c r="CM16" s="5">
-        <v>0.90731263160705566</v>
-      </c>
-      <c r="CN16" s="5">
-        <v>0.90782248973846436</v>
-      </c>
     </row>
-    <row r="17" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -5408,80 +4151,8 @@
       <c r="BP17" s="2">
         <v>33.858737945556641</v>
       </c>
-      <c r="BQ17" s="5">
-        <v>0.62507039308547974</v>
-      </c>
-      <c r="BR17" s="5">
-        <v>0.68395781517028809</v>
-      </c>
-      <c r="BS17" s="5">
-        <v>0.73052322864532471</v>
-      </c>
-      <c r="BT17" s="5">
-        <v>0.77590775489807129</v>
-      </c>
-      <c r="BU17" s="5">
-        <v>0.81062382459640503</v>
-      </c>
-      <c r="BV17" s="5">
-        <v>0.83909231424331665</v>
-      </c>
-      <c r="BW17" s="5">
-        <v>0.85849636793136597</v>
-      </c>
-      <c r="BX17" s="5">
-        <v>0.87118744850158691</v>
-      </c>
-      <c r="BY17" s="5">
-        <v>0.88372260332107544</v>
-      </c>
-      <c r="BZ17" s="5">
-        <v>0.89215826988220215</v>
-      </c>
-      <c r="CA17" s="5">
-        <v>0.89783453941345215</v>
-      </c>
-      <c r="CB17" s="5">
-        <v>0.90250366926193237</v>
-      </c>
-      <c r="CC17" s="5">
-        <v>0.90650719404220581</v>
-      </c>
-      <c r="CD17" s="5">
-        <v>0.90956223011016846</v>
-      </c>
-      <c r="CE17" s="5">
-        <v>0.9120669960975647</v>
-      </c>
-      <c r="CF17" s="5">
-        <v>0.9136505126953125</v>
-      </c>
-      <c r="CG17" s="5">
-        <v>0.91452896595001221</v>
-      </c>
-      <c r="CH17" s="5">
-        <v>0.91586750745773315</v>
-      </c>
-      <c r="CI17" s="5">
-        <v>0.91679024696350098</v>
-      </c>
-      <c r="CJ17" s="5">
-        <v>0.91745007038116455</v>
-      </c>
-      <c r="CK17" s="5">
-        <v>0.91858822107315063</v>
-      </c>
-      <c r="CL17" s="5">
-        <v>0.91924601793289185</v>
-      </c>
-      <c r="CM17" s="5">
-        <v>0.92001843452453613</v>
-      </c>
-      <c r="CN17" s="5">
-        <v>0.92061668634414673</v>
-      </c>
     </row>
-    <row r="18" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -5686,80 +4357,8 @@
       <c r="BP18" s="2">
         <v>33.831466674804688</v>
       </c>
-      <c r="BQ18" s="5">
-        <v>0.66094565391540527</v>
-      </c>
-      <c r="BR18" s="5">
-        <v>0.77099275588989258</v>
-      </c>
-      <c r="BS18" s="5">
-        <v>0.81927382946014404</v>
-      </c>
-      <c r="BT18" s="5">
-        <v>0.84916377067565918</v>
-      </c>
-      <c r="BU18" s="5">
-        <v>0.86978960037231445</v>
-      </c>
-      <c r="BV18" s="5">
-        <v>0.88515281677246094</v>
-      </c>
-      <c r="BW18" s="5">
-        <v>0.89571040868759155</v>
-      </c>
-      <c r="BX18" s="5">
-        <v>0.90347450971603394</v>
-      </c>
-      <c r="BY18" s="5">
-        <v>0.90961635112762451</v>
-      </c>
-      <c r="BZ18" s="5">
-        <v>0.91383540630340576</v>
-      </c>
-      <c r="CA18" s="5">
-        <v>0.91706633567810059</v>
-      </c>
-      <c r="CB18" s="5">
-        <v>0.91991734504699707</v>
-      </c>
-      <c r="CC18" s="5">
-        <v>0.92234641313552856</v>
-      </c>
-      <c r="CD18" s="5">
-        <v>0.92444992065429688</v>
-      </c>
-      <c r="CE18" s="5">
-        <v>0.92594307661056519</v>
-      </c>
-      <c r="CF18" s="5">
-        <v>0.92706173658370972</v>
-      </c>
-      <c r="CG18" s="5">
-        <v>0.92768067121505737</v>
-      </c>
-      <c r="CH18" s="5">
-        <v>0.92835003137588501</v>
-      </c>
-      <c r="CI18" s="5">
-        <v>0.92903298139572144</v>
-      </c>
-      <c r="CJ18" s="5">
-        <v>0.92950505018234253</v>
-      </c>
-      <c r="CK18" s="5">
-        <v>0.93030136823654175</v>
-      </c>
-      <c r="CL18" s="5">
-        <v>0.93081831932067871</v>
-      </c>
-      <c r="CM18" s="5">
-        <v>0.93141281604766846</v>
-      </c>
-      <c r="CN18" s="5">
-        <v>0.93174850940704346</v>
-      </c>
     </row>
-    <row r="19" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -5964,80 +4563,8 @@
       <c r="BP19" s="2">
         <v>29.697528839111332</v>
       </c>
-      <c r="BQ19" s="5">
-        <v>0.51196551322937012</v>
-      </c>
-      <c r="BR19" s="5">
-        <v>0.6152382493019104</v>
-      </c>
-      <c r="BS19" s="5">
-        <v>0.67794615030288696</v>
-      </c>
-      <c r="BT19" s="5">
-        <v>0.7280653715133667</v>
-      </c>
-      <c r="BU19" s="5">
-        <v>0.76649856567382813</v>
-      </c>
-      <c r="BV19" s="5">
-        <v>0.79639983177185059</v>
-      </c>
-      <c r="BW19" s="5">
-        <v>0.81965690851211548</v>
-      </c>
-      <c r="BX19" s="5">
-        <v>0.83546543121337891</v>
-      </c>
-      <c r="BY19" s="5">
-        <v>0.84888732433319092</v>
-      </c>
-      <c r="BZ19" s="5">
-        <v>0.85826194286346436</v>
-      </c>
-      <c r="CA19" s="5">
-        <v>0.86573433876037598</v>
-      </c>
-      <c r="CB19" s="5">
-        <v>0.87137424945831299</v>
-      </c>
-      <c r="CC19" s="5">
-        <v>0.87668037414550781</v>
-      </c>
-      <c r="CD19" s="5">
-        <v>0.88092190027236938</v>
-      </c>
-      <c r="CE19" s="5">
-        <v>0.88409692049026489</v>
-      </c>
-      <c r="CF19" s="5">
-        <v>0.88656264543533325</v>
-      </c>
-      <c r="CG19" s="5">
-        <v>0.88823831081390381</v>
-      </c>
-      <c r="CH19" s="5">
-        <v>0.88974446058273315</v>
-      </c>
-      <c r="CI19" s="5">
-        <v>0.89113795757293701</v>
-      </c>
-      <c r="CJ19" s="5">
-        <v>0.89223408699035645</v>
-      </c>
-      <c r="CK19" s="5">
-        <v>0.89411228895187378</v>
-      </c>
-      <c r="CL19" s="5">
-        <v>0.89507317543029785</v>
-      </c>
-      <c r="CM19" s="5">
-        <v>0.89600330591201782</v>
-      </c>
-      <c r="CN19" s="5">
-        <v>0.8969881534576416</v>
-      </c>
     </row>
-    <row r="20" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6242,80 +4769,8 @@
       <c r="BP20" s="2">
         <v>32.297107696533203</v>
       </c>
-      <c r="BQ20" s="5">
-        <v>0.61648964881896973</v>
-      </c>
-      <c r="BR20" s="5">
-        <v>0.67757105827331543</v>
-      </c>
-      <c r="BS20" s="5">
-        <v>0.72889047861099243</v>
-      </c>
-      <c r="BT20" s="5">
-        <v>0.77565479278564453</v>
-      </c>
-      <c r="BU20" s="5">
-        <v>0.80730831623077393</v>
-      </c>
-      <c r="BV20" s="5">
-        <v>0.83229494094848633</v>
-      </c>
-      <c r="BW20" s="5">
-        <v>0.85044169425964355</v>
-      </c>
-      <c r="BX20" s="5">
-        <v>0.86343652009963989</v>
-      </c>
-      <c r="BY20" s="5">
-        <v>0.87355571985244751</v>
-      </c>
-      <c r="BZ20" s="5">
-        <v>0.88094991445541382</v>
-      </c>
-      <c r="CA20" s="5">
-        <v>0.88735359907150269</v>
-      </c>
-      <c r="CB20" s="5">
-        <v>0.89193737506866455</v>
-      </c>
-      <c r="CC20" s="5">
-        <v>0.89609938859939575</v>
-      </c>
-      <c r="CD20" s="5">
-        <v>0.89924120903015137</v>
-      </c>
-      <c r="CE20" s="5">
-        <v>0.90191704034805298</v>
-      </c>
-      <c r="CF20" s="5">
-        <v>0.90358996391296387</v>
-      </c>
-      <c r="CG20" s="5">
-        <v>0.9048115611076355</v>
-      </c>
-      <c r="CH20" s="5">
-        <v>0.90608000755310059</v>
-      </c>
-      <c r="CI20" s="5">
-        <v>0.90750598907470703</v>
-      </c>
-      <c r="CJ20" s="5">
-        <v>0.9084937572479248</v>
-      </c>
-      <c r="CK20" s="5">
-        <v>0.90967833995819092</v>
-      </c>
-      <c r="CL20" s="5">
-        <v>0.91042888164520264</v>
-      </c>
-      <c r="CM20" s="5">
-        <v>0.9113507866859436</v>
-      </c>
-      <c r="CN20" s="5">
-        <v>0.91183161735534668</v>
-      </c>
     </row>
-    <row r="21" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6520,80 +4975,8 @@
       <c r="BP21" s="2">
         <v>33.851581573486328</v>
       </c>
-      <c r="BQ21" s="5">
-        <v>0.73172962665557861</v>
-      </c>
-      <c r="BR21" s="5">
-        <v>0.797210693359375</v>
-      </c>
-      <c r="BS21" s="5">
-        <v>0.82826697826385498</v>
-      </c>
-      <c r="BT21" s="5">
-        <v>0.85160839557647705</v>
-      </c>
-      <c r="BU21" s="5">
-        <v>0.86820745468139648</v>
-      </c>
-      <c r="BV21" s="5">
-        <v>0.88129603862762451</v>
-      </c>
-      <c r="BW21" s="5">
-        <v>0.89079666137695313</v>
-      </c>
-      <c r="BX21" s="5">
-        <v>0.89777946472167969</v>
-      </c>
-      <c r="BY21" s="5">
-        <v>0.90379375219345093</v>
-      </c>
-      <c r="BZ21" s="5">
-        <v>0.90774834156036377</v>
-      </c>
-      <c r="CA21" s="5">
-        <v>0.9114539623260498</v>
-      </c>
-      <c r="CB21" s="5">
-        <v>0.9139254093170166</v>
-      </c>
-      <c r="CC21" s="5">
-        <v>0.91626018285751343</v>
-      </c>
-      <c r="CD21" s="5">
-        <v>0.91851359605789185</v>
-      </c>
-      <c r="CE21" s="5">
-        <v>0.92004477977752686</v>
-      </c>
-      <c r="CF21" s="5">
-        <v>0.92095005512237549</v>
-      </c>
-      <c r="CG21" s="5">
-        <v>0.9217790961265564</v>
-      </c>
-      <c r="CH21" s="5">
-        <v>0.92249953746795654</v>
-      </c>
-      <c r="CI21" s="5">
-        <v>0.92345947027206421</v>
-      </c>
-      <c r="CJ21" s="5">
-        <v>0.9237934947013855</v>
-      </c>
-      <c r="CK21" s="5">
-        <v>0.92445576190948486</v>
-      </c>
-      <c r="CL21" s="5">
-        <v>0.92517197132110596</v>
-      </c>
-      <c r="CM21" s="5">
-        <v>0.92558550834655762</v>
-      </c>
-      <c r="CN21" s="5">
-        <v>0.92606914043426514</v>
-      </c>
     </row>
-    <row r="22" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6798,80 +5181,8 @@
       <c r="BP22" s="2">
         <v>31.35284423828125</v>
       </c>
-      <c r="BQ22" s="5">
-        <v>0.64760518074035645</v>
-      </c>
-      <c r="BR22" s="5">
-        <v>0.71908450126647949</v>
-      </c>
-      <c r="BS22" s="5">
-        <v>0.76532858610153198</v>
-      </c>
-      <c r="BT22" s="5">
-        <v>0.80098843574523926</v>
-      </c>
-      <c r="BU22" s="5">
-        <v>0.827475905418396</v>
-      </c>
-      <c r="BV22" s="5">
-        <v>0.84920239448547363</v>
-      </c>
-      <c r="BW22" s="5">
-        <v>0.86552906036376953</v>
-      </c>
-      <c r="BX22" s="5">
-        <v>0.87578600645065308</v>
-      </c>
-      <c r="BY22" s="5">
-        <v>0.88551509380340576</v>
-      </c>
-      <c r="BZ22" s="5">
-        <v>0.89197242259979248</v>
-      </c>
-      <c r="CA22" s="5">
-        <v>0.89720004796981812</v>
-      </c>
-      <c r="CB22" s="5">
-        <v>0.90108966827392578</v>
-      </c>
-      <c r="CC22" s="5">
-        <v>0.90443885326385498</v>
-      </c>
-      <c r="CD22" s="5">
-        <v>0.9074547290802002</v>
-      </c>
-      <c r="CE22" s="5">
-        <v>0.90978598594665527</v>
-      </c>
-      <c r="CF22" s="5">
-        <v>0.91121459007263184</v>
-      </c>
-      <c r="CG22" s="5">
-        <v>0.91231429576873779</v>
-      </c>
-      <c r="CH22" s="5">
-        <v>0.91322231292724609</v>
-      </c>
-      <c r="CI22" s="5">
-        <v>0.91442596912384033</v>
-      </c>
-      <c r="CJ22" s="5">
-        <v>0.91510415077209473</v>
-      </c>
-      <c r="CK22" s="5">
-        <v>0.91609543561935425</v>
-      </c>
-      <c r="CL22" s="5">
-        <v>0.91672641038894653</v>
-      </c>
-      <c r="CM22" s="5">
-        <v>0.91739016771316528</v>
-      </c>
-      <c r="CN22" s="5">
-        <v>0.91785812377929688</v>
-      </c>
     </row>
-    <row r="23" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7076,80 +5387,8 @@
       <c r="BP23" s="2">
         <v>32.115474700927727</v>
       </c>
-      <c r="BQ23" s="5">
-        <v>0.59657734632492065</v>
-      </c>
-      <c r="BR23" s="5">
-        <v>0.66480809450149536</v>
-      </c>
-      <c r="BS23" s="5">
-        <v>0.71110355854034424</v>
-      </c>
-      <c r="BT23" s="5">
-        <v>0.75481027364730835</v>
-      </c>
-      <c r="BU23" s="5">
-        <v>0.78768086433410645</v>
-      </c>
-      <c r="BV23" s="5">
-        <v>0.81303614377975464</v>
-      </c>
-      <c r="BW23" s="5">
-        <v>0.83199930191040039</v>
-      </c>
-      <c r="BX23" s="5">
-        <v>0.84677737951278687</v>
-      </c>
-      <c r="BY23" s="5">
-        <v>0.85766434669494629</v>
-      </c>
-      <c r="BZ23" s="5">
-        <v>0.8650936484336853</v>
-      </c>
-      <c r="CA23" s="5">
-        <v>0.87167954444885254</v>
-      </c>
-      <c r="CB23" s="5">
-        <v>0.8761444091796875</v>
-      </c>
-      <c r="CC23" s="5">
-        <v>0.88059496879577637</v>
-      </c>
-      <c r="CD23" s="5">
-        <v>0.88463807106018066</v>
-      </c>
-      <c r="CE23" s="5">
-        <v>0.88745760917663574</v>
-      </c>
-      <c r="CF23" s="5">
-        <v>0.88983958959579468</v>
-      </c>
-      <c r="CG23" s="5">
-        <v>0.89090496301651001</v>
-      </c>
-      <c r="CH23" s="5">
-        <v>0.89226615428924561</v>
-      </c>
-      <c r="CI23" s="5">
-        <v>0.89374649524688721</v>
-      </c>
-      <c r="CJ23" s="5">
-        <v>0.89446282386779785</v>
-      </c>
-      <c r="CK23" s="5">
-        <v>0.89596748352050781</v>
-      </c>
-      <c r="CL23" s="5">
-        <v>0.89676547050476074</v>
-      </c>
-      <c r="CM23" s="5">
-        <v>0.89763951301574707</v>
-      </c>
-      <c r="CN23" s="5">
-        <v>0.89848411083221436</v>
-      </c>
     </row>
-    <row r="24" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7354,80 +5593,8 @@
       <c r="BP24" s="2">
         <v>35.604671478271477</v>
       </c>
-      <c r="BQ24" s="5">
-        <v>0.77540630102157593</v>
-      </c>
-      <c r="BR24" s="5">
-        <v>0.83939814567565918</v>
-      </c>
-      <c r="BS24" s="5">
-        <v>0.86835324764251709</v>
-      </c>
-      <c r="BT24" s="5">
-        <v>0.88603466749191284</v>
-      </c>
-      <c r="BU24" s="5">
-        <v>0.89894890785217285</v>
-      </c>
-      <c r="BV24" s="5">
-        <v>0.90826743841171265</v>
-      </c>
-      <c r="BW24" s="5">
-        <v>0.91466468572616577</v>
-      </c>
-      <c r="BX24" s="5">
-        <v>0.92009884119033813</v>
-      </c>
-      <c r="BY24" s="5">
-        <v>0.92307174205780029</v>
-      </c>
-      <c r="BZ24" s="5">
-        <v>0.92562973499298096</v>
-      </c>
-      <c r="CA24" s="5">
-        <v>0.927295982837677</v>
-      </c>
-      <c r="CB24" s="5">
-        <v>0.92899173498153687</v>
-      </c>
-      <c r="CC24" s="5">
-        <v>0.93058151006698608</v>
-      </c>
-      <c r="CD24" s="5">
-        <v>0.93193793296813965</v>
-      </c>
-      <c r="CE24" s="5">
-        <v>0.93281912803649902</v>
-      </c>
-      <c r="CF24" s="5">
-        <v>0.93362700939178467</v>
-      </c>
-      <c r="CG24" s="5">
-        <v>0.93394577503204346</v>
-      </c>
-      <c r="CH24" s="5">
-        <v>0.93437492847442627</v>
-      </c>
-      <c r="CI24" s="5">
-        <v>0.93499183654785156</v>
-      </c>
-      <c r="CJ24" s="5">
-        <v>0.93522000312805176</v>
-      </c>
-      <c r="CK24" s="5">
-        <v>0.93565094470977783</v>
-      </c>
-      <c r="CL24" s="5">
-        <v>0.93612122535705566</v>
-      </c>
-      <c r="CM24" s="5">
-        <v>0.93632346391677856</v>
-      </c>
-      <c r="CN24" s="5">
-        <v>0.93658280372619629</v>
-      </c>
     </row>
-    <row r="25" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7632,80 +5799,8 @@
       <c r="BP25" s="2">
         <v>28.909074783325199</v>
       </c>
-      <c r="BQ25" s="5">
-        <v>0.56008332967758179</v>
-      </c>
-      <c r="BR25" s="5">
-        <v>0.64417010545730591</v>
-      </c>
-      <c r="BS25" s="5">
-        <v>0.70321094989776611</v>
-      </c>
-      <c r="BT25" s="5">
-        <v>0.75304234027862549</v>
-      </c>
-      <c r="BU25" s="5">
-        <v>0.79002892971038818</v>
-      </c>
-      <c r="BV25" s="5">
-        <v>0.81943774223327637</v>
-      </c>
-      <c r="BW25" s="5">
-        <v>0.8421790599822998</v>
-      </c>
-      <c r="BX25" s="5">
-        <v>0.85758614540100098</v>
-      </c>
-      <c r="BY25" s="5">
-        <v>0.87034064531326294</v>
-      </c>
-      <c r="BZ25" s="5">
-        <v>0.87947463989257813</v>
-      </c>
-      <c r="CA25" s="5">
-        <v>0.88660073280334473</v>
-      </c>
-      <c r="CB25" s="5">
-        <v>0.89174991846084595</v>
-      </c>
-      <c r="CC25" s="5">
-        <v>0.89670348167419434</v>
-      </c>
-      <c r="CD25" s="5">
-        <v>0.900562584400177</v>
-      </c>
-      <c r="CE25" s="5">
-        <v>0.90363091230392456</v>
-      </c>
-      <c r="CF25" s="5">
-        <v>0.90563446283340454</v>
-      </c>
-      <c r="CG25" s="5">
-        <v>0.90694165229797363</v>
-      </c>
-      <c r="CH25" s="5">
-        <v>0.90842503309249878</v>
-      </c>
-      <c r="CI25" s="5">
-        <v>0.90983039140701294</v>
-      </c>
-      <c r="CJ25" s="5">
-        <v>0.91094440221786499</v>
-      </c>
-      <c r="CK25" s="5">
-        <v>0.91226756572723389</v>
-      </c>
-      <c r="CL25" s="5">
-        <v>0.913280189037323</v>
-      </c>
-      <c r="CM25" s="5">
-        <v>0.91426634788513184</v>
-      </c>
-      <c r="CN25" s="5">
-        <v>0.91493523120880127</v>
-      </c>
     </row>
-    <row r="26" spans="1:92" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>51</v>
       </c>
@@ -7868,81 +5963,6 @@
       <c r="BP26" s="2">
         <v>32.301310777664177</v>
       </c>
-      <c r="BQ26" s="5">
-        <v>0.61023492366075516</v>
-      </c>
-      <c r="BR26" s="5">
-        <v>0.69015858322381973</v>
-      </c>
-      <c r="BS26" s="5">
-        <v>0.7400188917915026</v>
-      </c>
-      <c r="BT26" s="5">
-        <v>0.78037931521733606</v>
-      </c>
-      <c r="BU26" s="5">
-        <v>0.81139715760946274</v>
-      </c>
-      <c r="BV26" s="5">
-        <v>0.83597230911254883</v>
-      </c>
-      <c r="BW26" s="5">
-        <v>0.85384702434142434</v>
-      </c>
-      <c r="BX26" s="5">
-        <v>0.86653719345728553</v>
-      </c>
-      <c r="BY26" s="5">
-        <v>0.87719735254844033</v>
-      </c>
-      <c r="BZ26" s="5">
-        <v>0.88448943197727203</v>
-      </c>
-      <c r="CA26" s="5">
-        <v>0.8903626948595047</v>
-      </c>
-      <c r="CB26" s="5">
-        <v>0.8948042939106623</v>
-      </c>
-      <c r="CC26" s="5">
-        <v>0.89884264022111893</v>
-      </c>
-      <c r="CD26" s="5">
-        <v>0.90229844053586328</v>
-      </c>
-      <c r="CE26" s="5">
-        <v>0.90487070878346765</v>
-      </c>
-      <c r="CF26" s="5">
-        <v>0.90666056424379349</v>
-      </c>
-      <c r="CG26" s="5">
-        <v>0.90783788015445077</v>
-      </c>
-      <c r="CH26" s="5">
-        <v>0.90905549128850305</v>
-      </c>
-      <c r="CI26" s="5">
-        <v>0.91026195635398233</v>
-      </c>
-      <c r="CJ26" s="5">
-        <v>0.91109905391931534</v>
-      </c>
-      <c r="CK26" s="5">
-        <v>0.91231618076562881</v>
-      </c>
-      <c r="CL26" s="5">
-        <v>0.91321117927630746</v>
-      </c>
-      <c r="CM26" s="5">
-        <v>0.91401916990677512</v>
-      </c>
-      <c r="CN26" s="5">
-        <v>0.91461170464754105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:92" x14ac:dyDescent="0.3">
-      <c r="BQ28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>